<commit_message>
admin - data excel daftar rev
</commit_message>
<xml_diff>
--- a/public/Excel/Daftar.xlsx
+++ b/public/Excel/Daftar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\POLINEMA\SEMESTER 7\Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CACFF00-B279-4879-823B-A0E7F7B8E405}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F43ED0B4-C54F-4FA5-AA12-E5515375BBDF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4485" yWindow="1335" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2247" uniqueCount="1981">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2247" uniqueCount="1982">
   <si>
     <t>Nomor Urut</t>
   </si>
@@ -5974,6 +5974,9 @@
   </si>
   <si>
     <t>7P99</t>
+  </si>
+  <si>
+    <t>26P1</t>
   </si>
 </sst>
 </file>
@@ -6333,8 +6336,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H747"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+    <sheetView tabSelected="1" topLeftCell="B366" workbookViewId="0">
+      <selection activeCell="H370" sqref="H370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14720,7 +14723,7 @@
         <v>44916</v>
       </c>
       <c r="H370" t="s">
-        <v>1585</v>
+        <v>1981</v>
       </c>
     </row>
     <row r="371" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>